<commit_message>
placing the boxes by scanning the stack and calculating the colision mathmatically.
</commit_message>
<xml_diff>
--- a/Benchmarking.xlsx
+++ b/Benchmarking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\CY014-DC\Roaming Profiles\aserdyukov\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aserdyukov\source\repos\Algorithms-and-Data-Structures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A421922-D576-449B-9EAF-DE8D98D988E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE75532-FD6D-4F03-A004-9210F6E23BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>removeBox</t>
   </si>
@@ -52,11 +52,32 @@
   <si>
     <t>memset</t>
   </si>
+  <si>
+    <t>math</t>
+  </si>
+  <si>
+    <t>math+ reduce pointer addressing</t>
+  </si>
+  <si>
+    <t>same but return when collison</t>
+  </si>
+  <si>
+    <t>one if</t>
+  </si>
+  <si>
+    <t>no placeholders</t>
+  </si>
+  <si>
+    <t>with size_t</t>
+  </si>
+  <si>
+    <t>debugged</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,12 +113,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -1306,6 +1330,541 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$64:$E$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.0438800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.95628</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9559800000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9531799999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9491700000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9493499999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9546600000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.95608</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.94791</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9542299999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9762</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9719100000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.98163</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9662599999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9826699999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AEBA-41C5-97C3-54500CA33284}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$64:$F$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.9915499999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.91398</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8878900000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.88679</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.88409</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8853899999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.88486</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.89453</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8914200000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.88849</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.91612</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9188799999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.8897699999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.89055</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.89256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AEBA-41C5-97C3-54500CA33284}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$64:$G$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.2160500000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.13544</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.14097</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.13781</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.13662</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1320699999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.13374</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1353</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.13537</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.14113</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1456599999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1446700000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1372199999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1397299999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1415900000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AEBA-41C5-97C3-54500CA33284}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$64:$H$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.26353</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.14327</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.15161</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1510400000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1439600000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1391500000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1472599999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1573100000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1434800000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.14083</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.14324</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.16052</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1401300000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1431199999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1420999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-AEBA-41C5-97C3-54500CA33284}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$64:$I$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.3528800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.24319</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.23594</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2250700000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.22512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.22716</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2281899999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2260200000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.25779</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.24414</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.24404</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2408300000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2367699999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.22898</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.23092</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-AEBA-41C5-97C3-54500CA33284}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$64:$J$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.17666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1708799999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1158699999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1168800000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.11222</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1112299999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1108800000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1267199999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.11541</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1119399999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1113900000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1172500000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.11507</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.11209</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1115999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-AEBA-41C5-97C3-54500CA33284}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$64:$K$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.1893199999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.16259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1396200000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1582300000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1536500000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.13934</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1292899999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1341600000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1378200000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.13544</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.14815</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1300600000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1322399999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1332599999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.14655</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-AEBA-41C5-97C3-54500CA33284}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$64:$L$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-AEBA-41C5-97C3-54500CA33284}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$64:$M$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-AEBA-41C5-97C3-54500CA33284}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$64:$N$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-AEBA-41C5-97C3-54500CA33284}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1518,12 +2077,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>161921</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>14282</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>419096</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>52382</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4572000" cy="6053135"/>
+    <xdr:ext cx="4572000" cy="10044118"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 4">
@@ -1846,10 +2405,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A14:H80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A14:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="P90" sqref="P90"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2301,20 +2862,41 @@
         <v>0.847334864984431</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>4</v>
       </c>
       <c r="B63" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>6</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H63" t="s">
+        <v>9</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K63" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>3.4334099999999999</v>
       </c>
@@ -2327,8 +2909,29 @@
       <c r="D64">
         <v>2.27467</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>2.0438800000000001</v>
+      </c>
+      <c r="F64">
+        <v>1.9915499999999999</v>
+      </c>
+      <c r="G64">
+        <v>1.2160500000000001</v>
+      </c>
+      <c r="H64">
+        <v>1.26353</v>
+      </c>
+      <c r="I64">
+        <v>1.3528800000000001</v>
+      </c>
+      <c r="J64">
+        <v>1.17666</v>
+      </c>
+      <c r="K64">
+        <v>1.1893199999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>3.3449800000000001</v>
       </c>
@@ -2341,8 +2944,29 @@
       <c r="D65">
         <v>2.1798500000000001</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>1.95628</v>
+      </c>
+      <c r="F65">
+        <v>1.91398</v>
+      </c>
+      <c r="G65">
+        <v>1.13544</v>
+      </c>
+      <c r="H65">
+        <v>1.14327</v>
+      </c>
+      <c r="I65">
+        <v>1.24319</v>
+      </c>
+      <c r="J65">
+        <v>1.1708799999999999</v>
+      </c>
+      <c r="K65">
+        <v>1.16259</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>3.3207800000000001</v>
       </c>
@@ -2355,8 +2979,29 @@
       <c r="D66">
         <v>2.1703899999999998</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>1.9559800000000001</v>
+      </c>
+      <c r="F66">
+        <v>1.8878900000000001</v>
+      </c>
+      <c r="G66">
+        <v>1.14097</v>
+      </c>
+      <c r="H66">
+        <v>1.15161</v>
+      </c>
+      <c r="I66">
+        <v>1.23594</v>
+      </c>
+      <c r="J66">
+        <v>1.1158699999999999</v>
+      </c>
+      <c r="K66">
+        <v>1.1396200000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>3.3510900000000001</v>
       </c>
@@ -2369,8 +3014,29 @@
       <c r="D67">
         <v>2.1836199999999999</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>1.9531799999999999</v>
+      </c>
+      <c r="F67">
+        <v>1.88679</v>
+      </c>
+      <c r="G67">
+        <v>1.13781</v>
+      </c>
+      <c r="H67">
+        <v>1.1510400000000001</v>
+      </c>
+      <c r="I67">
+        <v>1.2250700000000001</v>
+      </c>
+      <c r="J67">
+        <v>1.1168800000000001</v>
+      </c>
+      <c r="K67">
+        <v>1.1582300000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>3.3370199999999999</v>
       </c>
@@ -2383,8 +3049,29 @@
       <c r="D68">
         <v>2.1677499999999998</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>1.9491700000000001</v>
+      </c>
+      <c r="F68">
+        <v>1.88409</v>
+      </c>
+      <c r="G68">
+        <v>1.13662</v>
+      </c>
+      <c r="H68">
+        <v>1.1439600000000001</v>
+      </c>
+      <c r="I68">
+        <v>1.22512</v>
+      </c>
+      <c r="J68">
+        <v>1.11222</v>
+      </c>
+      <c r="K68">
+        <v>1.1536500000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>3.3480699999999999</v>
       </c>
@@ -2397,8 +3084,29 @@
       <c r="D69">
         <v>2.17266</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>1.9493499999999999</v>
+      </c>
+      <c r="F69">
+        <v>1.8853899999999999</v>
+      </c>
+      <c r="G69">
+        <v>1.1320699999999999</v>
+      </c>
+      <c r="H69">
+        <v>1.1391500000000001</v>
+      </c>
+      <c r="I69">
+        <v>1.22716</v>
+      </c>
+      <c r="J69">
+        <v>1.1112299999999999</v>
+      </c>
+      <c r="K69">
+        <v>1.13934</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>3.3555100000000002</v>
       </c>
@@ -2411,8 +3119,29 @@
       <c r="D70">
         <v>2.17075</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>1.9546600000000001</v>
+      </c>
+      <c r="F70">
+        <v>1.88486</v>
+      </c>
+      <c r="G70">
+        <v>1.13374</v>
+      </c>
+      <c r="H70">
+        <v>1.1472599999999999</v>
+      </c>
+      <c r="I70">
+        <v>1.2281899999999999</v>
+      </c>
+      <c r="J70">
+        <v>1.1108800000000001</v>
+      </c>
+      <c r="K70">
+        <v>1.1292899999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>3.3448699999999998</v>
       </c>
@@ -2425,8 +3154,29 @@
       <c r="D71">
         <v>2.1770100000000001</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>1.95608</v>
+      </c>
+      <c r="F71">
+        <v>1.89453</v>
+      </c>
+      <c r="G71">
+        <v>1.1353</v>
+      </c>
+      <c r="H71">
+        <v>1.1573100000000001</v>
+      </c>
+      <c r="I71">
+        <v>1.2260200000000001</v>
+      </c>
+      <c r="J71">
+        <v>1.1267199999999999</v>
+      </c>
+      <c r="K71">
+        <v>1.1341600000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>3.3282600000000002</v>
       </c>
@@ -2439,8 +3189,29 @@
       <c r="D72">
         <v>2.2136499999999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>1.94791</v>
+      </c>
+      <c r="F72">
+        <v>1.8914200000000001</v>
+      </c>
+      <c r="G72">
+        <v>1.13537</v>
+      </c>
+      <c r="H72">
+        <v>1.1434800000000001</v>
+      </c>
+      <c r="I72">
+        <v>1.25779</v>
+      </c>
+      <c r="J72">
+        <v>1.11541</v>
+      </c>
+      <c r="K72">
+        <v>1.1378200000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>3.3471000000000002</v>
       </c>
@@ -2453,8 +3224,29 @@
       <c r="D73">
         <v>2.1672899999999999</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>1.9542299999999999</v>
+      </c>
+      <c r="F73">
+        <v>1.88849</v>
+      </c>
+      <c r="G73">
+        <v>1.14113</v>
+      </c>
+      <c r="H73">
+        <v>1.14083</v>
+      </c>
+      <c r="I73">
+        <v>1.24414</v>
+      </c>
+      <c r="J73">
+        <v>1.1119399999999999</v>
+      </c>
+      <c r="K73">
+        <v>1.13544</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>3.3596300000000001</v>
       </c>
@@ -2467,8 +3259,29 @@
       <c r="D74">
         <v>2.1772100000000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>1.9762</v>
+      </c>
+      <c r="F74">
+        <v>1.91612</v>
+      </c>
+      <c r="G74">
+        <v>1.1456599999999999</v>
+      </c>
+      <c r="H74">
+        <v>1.14324</v>
+      </c>
+      <c r="I74">
+        <v>1.24404</v>
+      </c>
+      <c r="J74">
+        <v>1.1113900000000001</v>
+      </c>
+      <c r="K74">
+        <v>1.14815</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>3.33969</v>
       </c>
@@ -2481,8 +3294,29 @@
       <c r="D75">
         <v>2.1713499999999999</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>1.9719100000000001</v>
+      </c>
+      <c r="F75">
+        <v>1.9188799999999999</v>
+      </c>
+      <c r="G75">
+        <v>1.1446700000000001</v>
+      </c>
+      <c r="H75">
+        <v>1.16052</v>
+      </c>
+      <c r="I75">
+        <v>1.2408300000000001</v>
+      </c>
+      <c r="J75">
+        <v>1.1172500000000001</v>
+      </c>
+      <c r="K75">
+        <v>1.1300600000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>3.3429099999999998</v>
       </c>
@@ -2495,8 +3329,29 @@
       <c r="D76">
         <v>2.1688900000000002</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>1.98163</v>
+      </c>
+      <c r="F76">
+        <v>1.8897699999999999</v>
+      </c>
+      <c r="G76">
+        <v>1.1372199999999999</v>
+      </c>
+      <c r="H76">
+        <v>1.1401300000000001</v>
+      </c>
+      <c r="I76">
+        <v>1.2367699999999999</v>
+      </c>
+      <c r="J76">
+        <v>1.11507</v>
+      </c>
+      <c r="K76">
+        <v>1.1322399999999999</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>3.3313799999999998</v>
       </c>
@@ -2509,8 +3364,29 @@
       <c r="D77">
         <v>2.1743700000000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>1.9662599999999999</v>
+      </c>
+      <c r="F77">
+        <v>1.89055</v>
+      </c>
+      <c r="G77">
+        <v>1.1397299999999999</v>
+      </c>
+      <c r="H77">
+        <v>1.1431199999999999</v>
+      </c>
+      <c r="I77">
+        <v>1.22898</v>
+      </c>
+      <c r="J77">
+        <v>1.11209</v>
+      </c>
+      <c r="K77">
+        <v>1.1332599999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>3.3372999999999999</v>
       </c>
@@ -2523,8 +3399,29 @@
       <c r="D78">
         <v>2.2000600000000001</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>1.9826699999999999</v>
+      </c>
+      <c r="F78">
+        <v>1.89256</v>
+      </c>
+      <c r="G78">
+        <v>1.1415900000000001</v>
+      </c>
+      <c r="H78">
+        <v>1.1420999999999999</v>
+      </c>
+      <c r="I78">
+        <v>1.23092</v>
+      </c>
+      <c r="J78">
+        <v>1.1115999999999999</v>
+      </c>
+      <c r="K78">
+        <v>1.14655</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79">
         <f>AVERAGE(A64:A78)</f>
         <v>3.3481333333333336</v>
@@ -2541,11 +3438,115 @@
         <f>AVERAGE(D64:D78)</f>
         <v>2.1846346666666667</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <f>AVERAGE(E64:E78)</f>
+        <v>1.9666259999999995</v>
+      </c>
+      <c r="F79">
+        <f t="shared" ref="F79:J79" si="2">AVERAGE(F64:F78)</f>
+        <v>1.9011246666666668</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="2"/>
+        <v>1.1435579999999999</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="2"/>
+        <v>1.1540366666666666</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="2"/>
+        <v>1.243136</v>
+      </c>
+      <c r="J79">
+        <f t="shared" si="2"/>
+        <v>1.1224060000000002</v>
+      </c>
+      <c r="K79">
+        <f t="shared" ref="K79" si="3">AVERAGE(K64:K78)</f>
+        <v>1.1446480000000001</v>
+      </c>
+      <c r="L79" t="e">
+        <f t="shared" ref="L79" si="4">AVERAGE(L64:L78)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M79" t="e">
+        <f t="shared" ref="M79" si="5">AVERAGE(M64:M78)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N79" t="e">
+        <f t="shared" ref="N79" si="6">AVERAGE(N64:N78)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O79" t="e">
+        <f t="shared" ref="O79" si="7">AVERAGE(O64:O78)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P79" t="e">
+        <f t="shared" ref="P79" si="8">AVERAGE(P64:P78)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B80">
         <f>($A$79/B79)-1</f>
         <v>0.51663857181942863</v>
+      </c>
+      <c r="C80">
+        <f t="shared" ref="C80:E80" si="9">($A$79/C79)-1</f>
+        <v>0.54702163988236707</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="9"/>
+        <v>0.53258271711029037</v>
+      </c>
+      <c r="E80">
+        <f>($A$79/E79)-1</f>
+        <v>0.70247588170467301</v>
+      </c>
+      <c r="F80">
+        <f t="shared" ref="F80:J80" si="10">($A$79/F79)-1</f>
+        <v>0.76113297146566228</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="10"/>
+        <v>1.9278211803278311</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="10"/>
+        <v>1.9012365291686288</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="10"/>
+        <v>1.6932960941790225</v>
+      </c>
+      <c r="J80">
+        <f t="shared" si="10"/>
+        <v>1.9829966458958102</v>
+      </c>
+      <c r="K80">
+        <f t="shared" ref="K80" si="11">($A$79/K79)-1</f>
+        <v>1.9250331397366991</v>
+      </c>
+      <c r="L80" t="e">
+        <f t="shared" ref="L80" si="12">($A$79/L79)-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M80" t="e">
+        <f t="shared" ref="M80" si="13">($A$79/M79)-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N80" t="e">
+        <f t="shared" ref="N80" si="14">($A$79/N79)-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O80" t="e">
+        <f t="shared" ref="O80" si="15">($A$79/O79)-1</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P80" t="e">
+        <f t="shared" ref="P80" si="16">($A$79/P79)-1</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned placeBox. Removed function boxArea from box struct. Removed depreciated functions. Func box collided improved if statement. Added box rotation. Improved for-statemt in the solveBox.
</commit_message>
<xml_diff>
--- a/Benchmarking.xlsx
+++ b/Benchmarking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aserdyukov\source\repos\Algorithms-and-Data-Structures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE75532-FD6D-4F03-A004-9210F6E23BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF7E6A2-0482-4159-A975-915DA0DAA01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>removeBox</t>
   </si>
@@ -73,11 +73,23 @@
   <si>
     <t>debugged</t>
   </si>
+  <si>
+    <t>Testing solution (200 000)</t>
+  </si>
+  <si>
+    <t>w + l outscoped</t>
+  </si>
+  <si>
+    <t>w + l + box outscoped</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -113,7 +125,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -122,6 +134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -2042,6 +2055,1182 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$114:$C$128</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.68667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71566799999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67990700000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66790300000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.66640699999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.67219899999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.66644099999999995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.66791</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.66289699999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.66132500000000005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.66357299999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.66561300000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.66548399999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.668381</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.66408900000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B5E-4F4E-A0A6-3DB74398D822}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$114:$D$128</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.69891400000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71042499999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.66745500000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.66861099999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.66834000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66741099999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.66855100000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.67114600000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.67419099999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.66906399999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.67073700000000003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.66954000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.66834099999999996</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.66709499999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.666408</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5B5E-4F4E-A0A6-3DB74398D822}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$114:$E$128</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.71040899999999996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69555</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.66455600000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.67558799999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.66880799999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.66607499999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.66429800000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.66543300000000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.66300000000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.66331200000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.68417600000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.66642500000000005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.66512899999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.67002200000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.66673400000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5B5E-4F4E-A0A6-3DB74398D822}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$114:$F$128</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.63449999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.636077</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.59847600000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.59717600000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59713499999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59902200000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.59486899999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.614622</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.597051</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.59391099999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.594696</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.59365699999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.59450000000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.59474899999999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.59539399999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5B5E-4F4E-A0A6-3DB74398D822}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$114:$G$128</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-5B5E-4F4E-A0A6-3DB74398D822}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$114:$H$128</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-5B5E-4F4E-A0A6-3DB74398D822}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$114:$I$128</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-5B5E-4F4E-A0A6-3DB74398D822}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="792946496"/>
+        <c:axId val="792946912"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="792946496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="792946912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="792946912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="792946496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
@@ -2106,6 +3295,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C5CDEE8-D1F3-1A3B-4AB6-08E617E47251}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2406,16 +3631,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A14:P80"/>
+  <dimension ref="A14:P130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="P90" sqref="P90"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="G136" sqref="G136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -3493,7 +4721,7 @@
         <v>0.51663857181942863</v>
       </c>
       <c r="C80">
-        <f t="shared" ref="C80:E80" si="9">($A$79/C79)-1</f>
+        <f t="shared" ref="C80:D80" si="9">($A$79/C79)-1</f>
         <v>0.54702163988236707</v>
       </c>
       <c r="D80">
@@ -3549,9 +4777,298 @@
         <v>#DIV/0!</v>
       </c>
     </row>
+    <row r="113" spans="1:6" s="3" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C114">
+        <v>0.68667</v>
+      </c>
+      <c r="D114">
+        <v>0.69891400000000004</v>
+      </c>
+      <c r="E114">
+        <v>0.71040899999999996</v>
+      </c>
+      <c r="F114">
+        <v>0.63449999999999995</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C115">
+        <v>0.71566799999999997</v>
+      </c>
+      <c r="D115">
+        <v>0.71042499999999997</v>
+      </c>
+      <c r="E115">
+        <v>0.69555</v>
+      </c>
+      <c r="F115">
+        <v>0.636077</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C116">
+        <v>0.67990700000000004</v>
+      </c>
+      <c r="D116">
+        <v>0.66745500000000002</v>
+      </c>
+      <c r="E116">
+        <v>0.66455600000000004</v>
+      </c>
+      <c r="F116">
+        <v>0.59847600000000001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C117">
+        <v>0.66790300000000002</v>
+      </c>
+      <c r="D117">
+        <v>0.66861099999999996</v>
+      </c>
+      <c r="E117">
+        <v>0.67558799999999997</v>
+      </c>
+      <c r="F117">
+        <v>0.59717600000000004</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C118">
+        <v>0.66640699999999997</v>
+      </c>
+      <c r="D118">
+        <v>0.66834000000000005</v>
+      </c>
+      <c r="E118">
+        <v>0.66880799999999996</v>
+      </c>
+      <c r="F118">
+        <v>0.59713499999999997</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C119">
+        <v>0.67219899999999999</v>
+      </c>
+      <c r="D119">
+        <v>0.66741099999999998</v>
+      </c>
+      <c r="E119">
+        <v>0.66607499999999997</v>
+      </c>
+      <c r="F119">
+        <v>0.59902200000000005</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C120">
+        <v>0.66644099999999995</v>
+      </c>
+      <c r="D120">
+        <v>0.66855100000000001</v>
+      </c>
+      <c r="E120">
+        <v>0.66429800000000006</v>
+      </c>
+      <c r="F120">
+        <v>0.59486899999999998</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C121">
+        <v>0.66791</v>
+      </c>
+      <c r="D121">
+        <v>0.67114600000000002</v>
+      </c>
+      <c r="E121">
+        <v>0.66543300000000005</v>
+      </c>
+      <c r="F121">
+        <v>0.614622</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C122">
+        <v>0.66289699999999996</v>
+      </c>
+      <c r="D122">
+        <v>0.67419099999999998</v>
+      </c>
+      <c r="E122">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="F122">
+        <v>0.597051</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C123">
+        <v>0.66132500000000005</v>
+      </c>
+      <c r="D123">
+        <v>0.66906399999999999</v>
+      </c>
+      <c r="E123">
+        <v>0.66331200000000001</v>
+      </c>
+      <c r="F123">
+        <v>0.59391099999999997</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C124">
+        <v>0.66357299999999997</v>
+      </c>
+      <c r="D124">
+        <v>0.67073700000000003</v>
+      </c>
+      <c r="E124">
+        <v>0.68417600000000001</v>
+      </c>
+      <c r="F124">
+        <v>0.594696</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C125">
+        <v>0.66561300000000001</v>
+      </c>
+      <c r="D125">
+        <v>0.66954000000000002</v>
+      </c>
+      <c r="E125">
+        <v>0.66642500000000005</v>
+      </c>
+      <c r="F125">
+        <v>0.59365699999999999</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C126">
+        <v>0.66548399999999996</v>
+      </c>
+      <c r="D126">
+        <v>0.66834099999999996</v>
+      </c>
+      <c r="E126">
+        <v>0.66512899999999997</v>
+      </c>
+      <c r="F126">
+        <v>0.59450000000000003</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C127">
+        <v>0.668381</v>
+      </c>
+      <c r="D127">
+        <v>0.66709499999999999</v>
+      </c>
+      <c r="E127">
+        <v>0.67002200000000001</v>
+      </c>
+      <c r="F127">
+        <v>0.59474899999999997</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C128">
+        <v>0.66408900000000004</v>
+      </c>
+      <c r="D128">
+        <v>0.666408</v>
+      </c>
+      <c r="E128">
+        <v>0.66673400000000005</v>
+      </c>
+      <c r="F128">
+        <v>0.59539399999999998</v>
+      </c>
+    </row>
+    <row r="129" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C129">
+        <f>AVERAGE(C114:C128)</f>
+        <v>0.67163113333333335</v>
+      </c>
+      <c r="D129">
+        <f>AVERAGE(D114:D128)</f>
+        <v>0.67374859999999992</v>
+      </c>
+      <c r="E129">
+        <f t="shared" ref="E129:J129" si="17">AVERAGE(E114:E128)</f>
+        <v>0.67263433333333333</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="17"/>
+        <v>0.60238900000000006</v>
+      </c>
+      <c r="G129" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H129" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I129" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J129" t="e">
+        <f t="shared" si="17"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="130" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C130" s="4">
+        <f>C129/200000</f>
+        <v>3.3581556666666668E-6</v>
+      </c>
+      <c r="D130" s="4">
+        <f t="shared" ref="D130:J130" si="18">D129/200000</f>
+        <v>3.3687429999999997E-6</v>
+      </c>
+      <c r="E130" s="4">
+        <f t="shared" si="18"/>
+        <v>3.3631716666666668E-6</v>
+      </c>
+      <c r="F130" s="4">
+        <f t="shared" si="18"/>
+        <v>3.0119450000000005E-6</v>
+      </c>
+      <c r="G130" s="4" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H130" s="4" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I130" s="4" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J130" s="4" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
-  <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Rotation works, but bug with an infinite loop.
</commit_message>
<xml_diff>
--- a/Benchmarking.xlsx
+++ b/Benchmarking.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aserdyukov\source\repos\Algorithms-and-Data-Structures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF7E6A2-0482-4159-A975-915DA0DAA01C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DEA9C2-5FF7-4D97-8F2E-CF14BD5F79A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>removeBox</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>w + l + box outscoped</t>
+  </si>
+  <si>
+    <t>placeBox cleaned</t>
+  </si>
+  <si>
+    <t>box rotation</t>
   </si>
 </sst>
 </file>
@@ -2430,6 +2436,51 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.60429699999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.62456999999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.575241</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58433000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59494499999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57751600000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.58143800000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.57629399999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.57653699999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.577874</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.58355400000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.58004299999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.59226400000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.57707799999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.58384999999999998</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2461,6 +2512,51 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.62042699999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.62805900000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.58841900000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58444399999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.59041900000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.59144799999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.58484000000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.59865699999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.58359899999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.58556900000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.58609800000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.58503400000000005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.58476399999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.58543100000000003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.58245199999999997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2494,6 +2590,51 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.60235799999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.60448000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55720400000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56044000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56119399999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.559087</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.56287200000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56090899999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.55694900000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.55547299999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.55716100000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55430599999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.55600700000000003</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.56038200000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.55524600000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2501,6 +2642,84 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-5B5E-4F4E-A0A6-3DB74398D822}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$114:$J$128</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.55508500000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54553799999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.55574699999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.530142</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.52453399999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.53100700000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.52936300000000003</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.52711399999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.52490499999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.52313200000000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.52520299999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.52642800000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.52447999999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.52779900000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.52764599999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7A99-4A3F-B859-64B13F405BBE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3297,14 +3516,14 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>108</xdr:row>
       <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>120</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
@@ -3633,8 +3852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A14:P130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="G136" sqref="G136"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="L125" sqref="L125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4777,7 +4996,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="113" spans="1:6" s="3" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" s="3" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>13</v>
       </c>
@@ -4787,8 +5006,14 @@
       <c r="E113" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="F113" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J113" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C114">
         <v>0.68667</v>
       </c>
@@ -4801,8 +5026,20 @@
       <c r="F114">
         <v>0.63449999999999995</v>
       </c>
+      <c r="G114">
+        <v>0.60429699999999997</v>
+      </c>
+      <c r="H114">
+        <v>0.62042699999999995</v>
+      </c>
+      <c r="I114">
+        <v>0.60235799999999995</v>
+      </c>
+      <c r="J114">
+        <v>0.55508500000000005</v>
+      </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C115">
         <v>0.71566799999999997</v>
       </c>
@@ -4815,8 +5052,20 @@
       <c r="F115">
         <v>0.636077</v>
       </c>
+      <c r="G115">
+        <v>0.62456999999999996</v>
+      </c>
+      <c r="H115">
+        <v>0.62805900000000003</v>
+      </c>
+      <c r="I115">
+        <v>0.60448000000000002</v>
+      </c>
+      <c r="J115">
+        <v>0.54553799999999997</v>
+      </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C116">
         <v>0.67990700000000004</v>
       </c>
@@ -4829,8 +5078,20 @@
       <c r="F116">
         <v>0.59847600000000001</v>
       </c>
+      <c r="G116">
+        <v>0.575241</v>
+      </c>
+      <c r="H116">
+        <v>0.58841900000000003</v>
+      </c>
+      <c r="I116">
+        <v>0.55720400000000003</v>
+      </c>
+      <c r="J116">
+        <v>0.55574699999999999</v>
+      </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C117">
         <v>0.66790300000000002</v>
       </c>
@@ -4843,8 +5104,20 @@
       <c r="F117">
         <v>0.59717600000000004</v>
       </c>
+      <c r="G117">
+        <v>0.58433000000000002</v>
+      </c>
+      <c r="H117">
+        <v>0.58444399999999996</v>
+      </c>
+      <c r="I117">
+        <v>0.56044000000000005</v>
+      </c>
+      <c r="J117">
+        <v>0.530142</v>
+      </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C118">
         <v>0.66640699999999997</v>
       </c>
@@ -4857,8 +5130,20 @@
       <c r="F118">
         <v>0.59713499999999997</v>
       </c>
+      <c r="G118">
+        <v>0.59494499999999995</v>
+      </c>
+      <c r="H118">
+        <v>0.59041900000000003</v>
+      </c>
+      <c r="I118">
+        <v>0.56119399999999997</v>
+      </c>
+      <c r="J118">
+        <v>0.52453399999999994</v>
+      </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C119">
         <v>0.67219899999999999</v>
       </c>
@@ -4871,8 +5156,20 @@
       <c r="F119">
         <v>0.59902200000000005</v>
       </c>
+      <c r="G119">
+        <v>0.57751600000000003</v>
+      </c>
+      <c r="H119">
+        <v>0.59144799999999997</v>
+      </c>
+      <c r="I119">
+        <v>0.559087</v>
+      </c>
+      <c r="J119">
+        <v>0.53100700000000001</v>
+      </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C120">
         <v>0.66644099999999995</v>
       </c>
@@ -4885,8 +5182,20 @@
       <c r="F120">
         <v>0.59486899999999998</v>
       </c>
+      <c r="G120">
+        <v>0.58143800000000001</v>
+      </c>
+      <c r="H120">
+        <v>0.58484000000000003</v>
+      </c>
+      <c r="I120">
+        <v>0.56287200000000004</v>
+      </c>
+      <c r="J120">
+        <v>0.52936300000000003</v>
+      </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C121">
         <v>0.66791</v>
       </c>
@@ -4899,8 +5208,20 @@
       <c r="F121">
         <v>0.614622</v>
       </c>
+      <c r="G121">
+        <v>0.57629399999999997</v>
+      </c>
+      <c r="H121">
+        <v>0.59865699999999999</v>
+      </c>
+      <c r="I121">
+        <v>0.56090899999999999</v>
+      </c>
+      <c r="J121">
+        <v>0.52711399999999997</v>
+      </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C122">
         <v>0.66289699999999996</v>
       </c>
@@ -4913,8 +5234,20 @@
       <c r="F122">
         <v>0.597051</v>
       </c>
+      <c r="G122">
+        <v>0.57653699999999997</v>
+      </c>
+      <c r="H122">
+        <v>0.58359899999999998</v>
+      </c>
+      <c r="I122">
+        <v>0.55694900000000003</v>
+      </c>
+      <c r="J122">
+        <v>0.52490499999999995</v>
+      </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C123">
         <v>0.66132500000000005</v>
       </c>
@@ -4927,8 +5260,20 @@
       <c r="F123">
         <v>0.59391099999999997</v>
       </c>
+      <c r="G123">
+        <v>0.577874</v>
+      </c>
+      <c r="H123">
+        <v>0.58556900000000001</v>
+      </c>
+      <c r="I123">
+        <v>0.55547299999999999</v>
+      </c>
+      <c r="J123">
+        <v>0.52313200000000004</v>
+      </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C124">
         <v>0.66357299999999997</v>
       </c>
@@ -4941,8 +5286,20 @@
       <c r="F124">
         <v>0.594696</v>
       </c>
+      <c r="G124">
+        <v>0.58355400000000002</v>
+      </c>
+      <c r="H124">
+        <v>0.58609800000000001</v>
+      </c>
+      <c r="I124">
+        <v>0.55716100000000002</v>
+      </c>
+      <c r="J124">
+        <v>0.52520299999999998</v>
+      </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C125">
         <v>0.66561300000000001</v>
       </c>
@@ -4955,8 +5312,20 @@
       <c r="F125">
         <v>0.59365699999999999</v>
       </c>
+      <c r="G125">
+        <v>0.58004299999999998</v>
+      </c>
+      <c r="H125">
+        <v>0.58503400000000005</v>
+      </c>
+      <c r="I125">
+        <v>0.55430599999999997</v>
+      </c>
+      <c r="J125">
+        <v>0.52642800000000001</v>
+      </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C126">
         <v>0.66548399999999996</v>
       </c>
@@ -4969,8 +5338,20 @@
       <c r="F126">
         <v>0.59450000000000003</v>
       </c>
+      <c r="G126">
+        <v>0.59226400000000001</v>
+      </c>
+      <c r="H126">
+        <v>0.58476399999999995</v>
+      </c>
+      <c r="I126">
+        <v>0.55600700000000003</v>
+      </c>
+      <c r="J126">
+        <v>0.52447999999999995</v>
+      </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C127">
         <v>0.668381</v>
       </c>
@@ -4983,8 +5364,20 @@
       <c r="F127">
         <v>0.59474899999999997</v>
       </c>
+      <c r="G127">
+        <v>0.57707799999999998</v>
+      </c>
+      <c r="H127">
+        <v>0.58543100000000003</v>
+      </c>
+      <c r="I127">
+        <v>0.56038200000000005</v>
+      </c>
+      <c r="J127">
+        <v>0.52779900000000002</v>
+      </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C128">
         <v>0.66408900000000004</v>
       </c>
@@ -4996,6 +5389,18 @@
       </c>
       <c r="F128">
         <v>0.59539399999999998</v>
+      </c>
+      <c r="G128">
+        <v>0.58384999999999998</v>
+      </c>
+      <c r="H128">
+        <v>0.58245199999999997</v>
+      </c>
+      <c r="I128">
+        <v>0.55524600000000002</v>
+      </c>
+      <c r="J128">
+        <v>0.52764599999999995</v>
       </c>
     </row>
     <row r="129" spans="3:10" x14ac:dyDescent="0.25">
@@ -5015,21 +5420,17 @@
         <f t="shared" si="17"/>
         <v>0.60238900000000006</v>
       </c>
-      <c r="G129" t="e">
+      <c r="G129">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H129" t="e">
+        <v>0.58598873333333334</v>
+      </c>
+      <c r="H129">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I129" t="e">
+        <v>0.59197733333333324</v>
+      </c>
+      <c r="I129">
         <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J129" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <v>0.56427119999999997</v>
       </c>
     </row>
     <row r="130" spans="3:10" x14ac:dyDescent="0.25">
@@ -5049,21 +5450,21 @@
         <f t="shared" si="18"/>
         <v>3.0119450000000005E-6</v>
       </c>
-      <c r="G130" s="4" t="e">
+      <c r="G130" s="4">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H130" s="4" t="e">
+        <v>2.9299436666666669E-6</v>
+      </c>
+      <c r="H130" s="4">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I130" s="4" t="e">
+        <v>2.9598866666666661E-6</v>
+      </c>
+      <c r="I130" s="4">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J130" s="4" t="e">
+        <v>2.8213559999999998E-6</v>
+      </c>
+      <c r="J130" s="4">
         <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>